<commit_message>
all has permission as admin for simulation purpose only
</commit_message>
<xml_diff>
--- a/storage/app/import/sim-user.xlsx
+++ b/storage/app/import/sim-user.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t xml:space="preserve">nrp</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">arifin</t>
   </si>
   <si>
-    <t xml:space="preserve">engineer</t>
+    <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">zainal.arifin@ptmmf.co.id</t>
@@ -91,9 +91,6 @@
     <t xml:space="preserve">raharjo</t>
   </si>
   <si>
-    <t xml:space="preserve">helper</t>
-  </si>
-  <si>
     <t xml:space="preserve">widodo@ptmmf.co.id</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
     <t xml:space="preserve">julianto</t>
   </si>
   <si>
-    <t xml:space="preserve">ppic</t>
-  </si>
-  <si>
     <t xml:space="preserve">julianto@ptmmf.co.id</t>
   </si>
   <si>
@@ -241,9 +235,6 @@
     <t xml:space="preserve">Wahyudi</t>
   </si>
   <si>
-    <t xml:space="preserve">Manager</t>
-  </si>
-  <si>
     <t xml:space="preserve">muhwahyudi@ptmmf.co.id</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t xml:space="preserve">Eka</t>
   </si>
   <si>
-    <t xml:space="preserve">Staff</t>
-  </si>
-  <si>
     <t xml:space="preserve">winda.eka@ptmmf.co.id </t>
   </si>
   <si>
@@ -274,9 +262,6 @@
     <t xml:space="preserve">Andreawan</t>
   </si>
   <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
     <t xml:space="preserve">dika@ptmmf.co.id </t>
   </si>
   <si>
@@ -308,9 +293,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sanjaya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marketing</t>
   </si>
   <si>
     <t xml:space="preserve">aldi@ptmmf.co.id </t>
@@ -515,10 +497,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,7 +531,7 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="X1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -575,7 +557,7 @@
       <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="X2" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -590,19 +572,19 @@
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="X3" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,16 +592,16 @@
         <v>18040067</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>12</v>
@@ -627,8 +609,8 @@
       <c r="G4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="0" t="s">
-        <v>24</v>
+      <c r="X4" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,16 +618,16 @@
         <v>18040071</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>12</v>
@@ -653,8 +635,8 @@
       <c r="G5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y5" s="0" t="s">
-        <v>28</v>
+      <c r="X5" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,16 +644,16 @@
         <v>18040073</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>12</v>
@@ -679,8 +661,8 @@
       <c r="G6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y6" s="0" t="s">
-        <v>31</v>
+      <c r="X6" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,16 +670,16 @@
         <v>18040059</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>12</v>
@@ -705,8 +687,8 @@
       <c r="G7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y7" s="0" t="s">
-        <v>35</v>
+      <c r="X7" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,16 +696,16 @@
         <v>19010087</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>12</v>
@@ -731,8 +713,8 @@
       <c r="G8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y8" s="0" t="s">
-        <v>39</v>
+      <c r="X8" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,16 +722,16 @@
         <v>18040074</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>12</v>
@@ -757,8 +739,8 @@
       <c r="G9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y9" s="0" t="s">
-        <v>43</v>
+      <c r="X9" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,16 +748,16 @@
         <v>18040070</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>12</v>
@@ -783,8 +765,8 @@
       <c r="G10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y10" s="0" t="s">
-        <v>47</v>
+      <c r="X10" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,16 +774,16 @@
         <v>18040069</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>50</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>12</v>
@@ -809,8 +791,8 @@
       <c r="G11" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y11" s="0" t="s">
-        <v>51</v>
+      <c r="X11" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,16 +800,16 @@
         <v>18040075</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>12</v>
@@ -835,8 +817,8 @@
       <c r="G12" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y12" s="0" t="s">
-        <v>55</v>
+      <c r="X12" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,16 +826,16 @@
         <v>19040121</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>12</v>
@@ -861,8 +843,8 @@
       <c r="G13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Y13" s="0" t="s">
-        <v>59</v>
+      <c r="X13" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,25 +852,25 @@
         <v>18110085</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="X14" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y14" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,25 +878,25 @@
         <v>18180085</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="F15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="X15" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y15" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,25 +904,25 @@
         <v>19040113</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="X16" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y16" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,22 +930,22 @@
         <v>19040127</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,22 +953,22 @@
         <v>19040126</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="F18" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,22 +976,22 @@
         <v>17040025</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,22 +999,22 @@
         <v>19040125</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,28 +1022,28 @@
         <v>19060129</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D21" type="list">
-      <formula1>$Y$1:$Y$16</formula1>
+      <formula1>$X$1:$X$16</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>